<commit_message>
Completed person-date logic - complete prototype 1
</commit_message>
<xml_diff>
--- a/data/TestFile.xlsx
+++ b/data/TestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28044358-95AE-4C07-9814-CE53D46A5922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F349887E-972D-49A6-AD66-BD28A1C58132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,8 +639,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1103,7 @@
         <v>2944000</v>
       </c>
       <c r="F19" s="11">
-        <v>44719</v>
+        <v>44718</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>9</v>

</xml_diff>